<commit_message>
been a while, many many things have been updated all of which I cannot really remember, ah well. JP
</commit_message>
<xml_diff>
--- a/Demo/Weather and Properties/Test WTG Properties.xlsx
+++ b/Demo/Weather and Properties/Test WTG Properties.xlsx
@@ -2247,7 +2247,12 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5fb5e84a-5684-468e-b345-7aeeb4845130">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c891a41a-a233-45b7-a3f1-ec06333a8c94" xsi:nil="true"/>
+  </documentManagement>
 </p:properties>
 </file>
 
@@ -2261,8 +2266,8 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BE91B0E0F707B44ADD54BD807FC8041" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2343359116c41cd6df5e9933b71ba69e">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c891a41a-a233-45b7-a3f1-ec06333a8c94" xmlns:ns3="5fb5e84a-5684-468e-b345-7aeeb4845130" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5bf6b77a57d9afd5d212f0342177a31b" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000BE91B0E0F707B44ADD54BD807FC8041" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="aaf53faa0b720e0e3b2b5121d0fe8108">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c891a41a-a233-45b7-a3f1-ec06333a8c94" xmlns:ns3="5fb5e84a-5684-468e-b345-7aeeb4845130" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88a8651ba02bfcc8abd053d50e01d782" ns2:_="" ns3:_="">
     <xsd:import namespace="c891a41a-a233-45b7-a3f1-ec06333a8c94"/>
     <xsd:import namespace="5fb5e84a-5684-468e-b345-7aeeb4845130"/>
     <xsd:element name="properties">
@@ -2283,6 +2288,9 @@
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns2:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2318,6 +2326,17 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{ae301ee1-5209-4650-b0c1-2c09e3e2885c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="c891a41a-a233-45b7-a3f1-ec06333a8c94">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="5fb5e84a-5684-468e-b345-7aeeb4845130" elementFormDefault="qualified">
@@ -2376,6 +2395,18 @@
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="20" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="bdf4d8d7-af3c-42ab-a689-3e7dc994f6b2" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -2503,20 +2534,5 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{116097D9-7762-4AAE-AB7C-C0595249B871}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="c891a41a-a233-45b7-a3f1-ec06333a8c94"/>
-    <ds:schemaRef ds:uri="5fb5e84a-5684-468e-b345-7aeeb4845130"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B636DBC4-DCEA-42D2-924C-CBB99CC00617}"/>
 </file>
</xml_diff>